<commit_message>
Changed wording in base.xlsx for Contributed worksheet
</commit_message>
<xml_diff>
--- a/excelworkbook/base.xlsx
+++ b/excelworkbook/base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Scripts\Server47\excelworkbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEB4253-A8D0-4624-B503-BC1B31F2A66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D82F2E-C76B-44E3-850C-910A5BDE4F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22755" yWindow="6255" windowWidth="20505" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22755" yWindow="6255" windowWidth="20505" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Cash Left</t>
   </si>
@@ -85,18 +85,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Contributed</t>
-  </si>
-  <si>
-    <t>YTD Principal Contributed</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -140,6 +128,12 @@
   </si>
   <si>
     <t>Close Price</t>
+  </si>
+  <si>
+    <t>Total Principal Contributed</t>
+  </si>
+  <si>
+    <t>CONTRIBUTED</t>
   </si>
 </sst>
 </file>
@@ -444,6 +438,182 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
@@ -472,182 +642,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border>
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.1498764000366222"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
@@ -692,26 +686,26 @@
     <sortCondition descending="1" ref="G4:G8"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Shares" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Shares" dataDxfId="8">
       <calculatedColumnFormula>IF(A5="","",SUMIFS(Transactions!$E$2:$E$200,Transactions!$B$2:$B$200,A5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Money Invested" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Money Invested" dataDxfId="7">
       <calculatedColumnFormula>IF(A5="","",SUMIFS(Transactions!F2:F200,Transactions!B2:B200,A5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Mkt Value" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Mkt Value" dataDxfId="6">
       <calculatedColumnFormula>IF(A5="","",SUM(G5*B5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Percent Change" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Percent Change" dataDxfId="5">
       <calculatedColumnFormula>IF(A5="","",SUM(D5-C5) / C5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Gain" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Gain" dataDxfId="4">
       <calculatedColumnFormula>IF(A5="","",D5-C5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Current Share Price" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Current Share Price" dataDxfId="3">
       <calculatedColumnFormula>IF(A5="","",SUMIFS('Position Data'!$D$2:$D$200,'Position Data'!$A$2:$A$200,A5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Percent of Total Investment" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Percent of Total Investment" dataDxfId="2">
       <calculatedColumnFormula>IF(A5="","",C5/$E$2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -984,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E11" sqref="E11"/>
     </sheetView>
@@ -1300,22 +1294,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>E5&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>E6&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>E7&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>E5&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1331,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,17 +1347,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D1" s="23" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E1" s="2"/>
       <c r="I1" s="6"/>
@@ -1472,9 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1487,22 +1479,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1725,7 +1717,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1738,19 +1730,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1879,28 +1871,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>